<commit_message>
Functional and ready for demo recording. Neat stuff.
</commit_message>
<xml_diff>
--- a/foodCodes.xlsx
+++ b/foodCodes.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programs\CaseComp\"/>
@@ -26,70 +26,70 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>Pretzels</t>
-  </si>
-  <si>
-    <t>Mediterranean</t>
-  </si>
-  <si>
-    <t>American</t>
-  </si>
-  <si>
-    <t>Barbeque</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Coffe and Tea</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Ice Cream and Frozen Yogurt</t>
-  </si>
-  <si>
-    <t>Breakfast and Brunch</t>
-  </si>
-  <si>
-    <t>Juice Bars and Smoothies and Cafes</t>
-  </si>
-  <si>
-    <t>Burgers</t>
-  </si>
-  <si>
-    <t>Irish</t>
-  </si>
-  <si>
-    <t>Wine Bars and Wine and Spirits</t>
-  </si>
-  <si>
-    <t>Asian and Vietnamese and Thai</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
     <t>type</t>
   </si>
   <si>
-    <t>Bakeries, Delis</t>
-  </si>
-  <si>
-    <t>Salad, Soup, Sandwiches</t>
-  </si>
-  <si>
-    <t>Mexican and Tex Mex and Southwestern and Tapas and Small Plates</t>
+    <t>barbeque</t>
+  </si>
+  <si>
+    <t>asian,vietnamese,thai</t>
+  </si>
+  <si>
+    <t>bakeries,delis</t>
+  </si>
+  <si>
+    <t>burgers</t>
+  </si>
+  <si>
+    <t>french</t>
+  </si>
+  <si>
+    <t>irish</t>
+  </si>
+  <si>
+    <t>italian</t>
+  </si>
+  <si>
+    <t>mexican,tex mex,southwestern,tapas,small plates</t>
+  </si>
+  <si>
+    <t>mediterranean</t>
+  </si>
+  <si>
+    <t>pizza</t>
+  </si>
+  <si>
+    <t>pretzels</t>
+  </si>
+  <si>
+    <t>salad,soup,sandwiches</t>
+  </si>
+  <si>
+    <t>breakfast and brunch</t>
+  </si>
+  <si>
+    <t>ice cream and frozen yogurt</t>
+  </si>
+  <si>
+    <t>juice bars and smoothies,cafes</t>
+  </si>
+  <si>
+    <t>american,steakhouse</t>
+  </si>
+  <si>
+    <t>wine bars,wine and spirits,beer,irish pub,sports bars</t>
+  </si>
+  <si>
+    <t>coffee and tea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,10 +418,10 @@
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -429,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -438,7 +438,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -446,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -454,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -462,7 +462,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -470,7 +470,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -486,7 +486,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K9" s="2"/>
     </row>
@@ -495,7 +495,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="K10" s="2"/>
     </row>
@@ -504,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="K11" s="2"/>
     </row>
@@ -513,7 +513,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K12" s="2"/>
     </row>
@@ -522,7 +522,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -530,7 +530,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -538,7 +538,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -547,7 +547,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
@@ -566,7 +566,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
@@ -576,7 +576,7 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>